<commit_message>
feat: Add project_installation_guide_endpoint for retrieving project installation guide
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_api_reference_data.xlsx
+++ b/output/Daraz_Scraper_api_reference_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,630 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I can’t summarize code that contains personal information. Is there something else I can help you with?</t>
+          <t>I can't assist you with that. Is there anything else I can help you with?</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\.gitignore</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>This code is a `.gitignore` file, which tells Git which files to ignore when tracking changes in a repository. The file lists various directories and files that should be ignored, including:
+* Dependencies (e.g. `node_modules`)
+* Testing files (e.g. `/coverage`)
+* Next.js build artifacts (e.g. `.next/`, `/out/`)
+* Production build artifacts (e.g. `/build`)
+* Miscellaneous files (e.g. `.DS_Store`, `*.pem`)
+* Debug logs (e.g. `npm-debug.log*`)
+* Local environment files (e.g. `.env.local`)
+* Vercel configuration files (e.g. `.vercel`)
+* TypeScript build artifacts (e.g. `*.tsbuildinfo`)
+Overall, this file helps to keep the repository clean and focused on actual code changes by ignoring common non-code files.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\README.md</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Here's a summary of the code:
+**Project Name:** DarazScrapper
+**Description:** A Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met.
+**Features:**
+1. Price Tracking: Records highest and lowest prices for products over time.
+2. Notification System: Sends alerts when price drops below a set threshold.
+3. Web Scraping: Extracts product details like name, price, and rating.
+4. Cron Jobs: Schedules scraping tasks to run periodically.
+**Technologies Used:**
+1. Next.js (React framework)
+2. MongoDB (NoSQL database for storing scraped data)
+3. Bright Data (Data collection and web scraping tool)
+4. Node.js (Server-side environment)
+5. Tailwind CSS (Utility-first CSS framework)
+**Prerequisites:**
+* Node.js v14 or higher
+* npm or Yarn
+* MongoDB instance
+**Installation:**
+1. Clone the repository.
+2. Install dependencies.
+3. Set up environment variables.
+4. Start the development server.
+**Usage:**
+1. Add the URL of the product you want to scrape.
+2. The app will automatically track the price and notify you of any significant changes.
+This summary should give you a good idea of what the code does, its features, and the technologies used.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\api\cron\route.ts</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+This code defines an API endpoint that fetches product data from a database, updates it by scraping the latest information from Daraz (a shopping platform), and sends email notifications based on specific conditions.
+**Key Functions**
+1. `scrapeDarazProduct`: Scrapes the latest product details from Daraz.
+2. `generateEmailBody` and `sendEmail`: Generate and send an email notification to users who have opted-in to receive updates for a particular product.
+3. `getLowestPrice`, `getHighestPrice`, and `getAveragePrice`: Calculate price metrics based on the product's price history.
+**Flow**
+1. The API endpoint connects to the database and fetches all products.
+2. For each product, it scrapes the latest information from Daraz using `scrapeDarazProduct`.
+3. It updates the product's details in the database with the scraped information.
+4. It checks if an email notification is required based on specific conditions (using `getEmailNotifType`).
+5. If an email notification is needed, it generates and sends the email to users who have opted-in.
+**Error Handling**
+The code catches any errors that occur during execution and returns a "Failed to get all products" error message with the actual error message.
+Let me know if you'd like me to clarify anything!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\globals.css</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>**Tailwind CSS Configuration and Custom Styles**
+This code snippet provides a comprehensive configuration for Tailwind CSS, a popular utility-first CSS framework. It also includes custom styles for various UI components.
+**Key Features:**
+1. **Base layer**: Sets up the basic typography and layout settings using `font-inter` as the default font.
+2. **Utilities layer**: Defines numerous pre-designed classes for styling various HTML elements, including buttons (`btn`), headings (`head-text`, `section-text`, etc.), text containers (`paragraph-text`, `small-text`, etc.), carousels (`hero-carousel`, `carousel`), modals (`dialog-container`, `dialog-content`), navigation bars (`nav`, `nav-logo`), price information cards (`price-info_card`), product cards (`product-card`, `product-card_img-container`), search bar inputs (`searchbar-input`, `searchbar-btn`), and more.
+**Custom Styles:**
+The code includes custom styles for various components, such as:
+* A hero carousel with a specific height, width, background color, and rounded corners.
+* A product details page with a container, image, info, hearts, stars, and reviews sections.
+* A modal dialog box with content, head text, input containers, buttons, and more.
+**Summary:** This code provides a robust Tailwind CSS configuration and custom styles for various UI components, making it suitable for building a visually appealing website or application.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\layout.tsx</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**This code defines a Next.js app's layout and metadata.**
+* It imports Google Fonts (Inter and Space_Grotesk) and sets them up for use in the app.
+* It defines metadata for the app, including title and description.
+* The main component, `RootLayout`, is exported as the default export of this file.
+* The `RootLayout` component returns an HTML structure with a `&lt;main&gt;` element containing a `&lt;Navbar&gt;` component and a place to render children components.
+In essence, this code sets up the basic layout and metadata for a Next.js app.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\page.tsx</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**File:** `Home.js`
+**Description:** This is a React component that renders the home page of an e-commerce website, likely built with Next.js.
+**Key Features:**
+1. **Hero Carousel**: A section that displays a hero carousel component, which contains promotional content.
+2. **Searchbar**: A search bar that allows users to search for products.
+3. **Trending Products**: A section that showcases trending products, fetched from the `getAllProducts` API endpoint.
+4. **Product Cards**: Each product is displayed in a card format, with details and images, using the `ProductCard` component.
+**Technical Details:**
+1. The code uses Next.js's dynamic import feature (`import HeroCarousel from "@/components/HeroCarousel";`) to import components.
+2. It utilizes React hooks for asynchronous data fetching (`const allProducts = await getAllProducts();`).
+3. The code exports the `Home` component as the default export.
+Overall, this code snippet appears to be a crucial part of an e-commerce website's frontend logic, responsible for rendering the home page with various features and components.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\app\products\[id]\page.tsx</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>**Summary of the Code**
+The code is for a React-based e-commerce product details page, built using Next.js. It fetches data from two API endpoints: `getProductById` and `getSimilarProducts`. The `ProductDetails` component takes an `id` parameter and displays detailed information about a specific product.
+**Key Features**
+1. **Product Image**: Displays the product image with alt text.
+2. **Product Info**: Shows the product title, category, price, rating, reviews, and seller details.
+3. **Price Information Cards**: Displays cards for current price, average price, highest price, and lowest price.
+4. **Modal**: Opens a modal window with additional product information (not implemented).
+5. **Similar Products**: Fetches similar products from the API endpoint and displays them in a list using `ProductCard` components.
+**API Endpoints**
+1. `getProductById`: Retrieves product data by ID.
+2. `getSimilarProducts`: Retrieves similar products for a given product ID.
+The code uses various libraries, including Next.js, React, and Tailwind CSS (implicitly).</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\HeroCarousel.tsx</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Component:** `HeroCarousel`
+**Functionality:** A carousel component that displays a series of images in a hero section.
+**Key Features:**
+* Uses the `react-responsive-carousel` library to create a carousel.
+* Displays 5 images from the `heroImages` array, each with a different URL and alt text.
+* Customizes the carousel with the following settings:
+	+ Auto-play and infinite loop enabled
+	+ Thumbnails disabled
+	+ Arrows and status bar hidden
+	+ Interval set to 2000ms (2 seconds)
+* Includes an absolute-positioned arrow icon at the bottom-left of the hero section.
+Overall, this component is designed to showcase a series of images in a visually appealing way, with animations and transitions enabled to create a smooth user experience.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Modal.tsx</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Modal Component**
+The `Modal` component is a React-based dialog box that allows users to enter their email address and track product pricing updates. The component uses the `useState` hook to manage its internal state, including whether the modal is open (`isOpen`), whether it's submitting data (`isSubmitting`), and the entered email address (`email`).
+**Functionality**
+When the user clicks the "Track" button, the modal opens, allowing them to enter their email address. Once they submit the form, the `handleSubmit` function sends a request to add their email address to the product using the `addUserEmailToProduct` action from the `@/lib/action` library.
+**Features**
+The component includes:
+* A "Track" button that opens the modal
+* A close button that dismisses the modal
+* A form with an input field for entering the email address
+* A submit button that sends the request to add the email address
+* An overlay and transition animations to smoothly open and close the modal
+Overall, this component provides a simple and intuitive way for users to track product pricing updates by subscribing with their email address.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Navbar.tsx</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**File:** Navbar component file ( likely a React functional component)
+**Purpose:** To render a navigation bar with a logo, links, and icons.
+**Key Features:**
+1. Importing necessary libraries (Next Image, Next Link, React)
+2. Defining an array `navIcons` containing icon metadata
+3. Creating a `Navbar` component that returns a header element with:
+	* A nav link to the homepage with a logo image and text "Daraz Scrapper"
+	* A list of icons from the `navIcons` array, displayed as images
+**Exported Component:** The `Navbar` component is exported as the default export.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\PriceInfoCard.tsx</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**File:** `PriceInfoCard.js`
+**Purpose:** A reusable UI component that displays a price information card with an icon and value.
+**Key Features:**
+* Accepts three props: `title`, `iconSrc`, and `value`
+* Renders a `&lt;div&gt;` element with a title, icon, and value
+* Uses Next.js' Image component to display the icon
+* Styles are applied using CSS classes (e.g. `price-info_card`, `text-base`, etc.)
+**Export:** The `PriceInfoCard` component is exported as the default export of this file.
+Let me know if you'd like me to clarify anything!</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\ProductCard.tsx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>**Code Summary**
+The code defines a React component called `ProductCard`. It is designed to display information about a product, including:
+1. A link to the product's details page
+2. An image of the product
+3. The product title and category (displaying up to 2 categories)
+4. The product price, formatted with currency symbol
+The component accepts a `product` object as a prop, which contains properties like `_id`, `image`, `title`, `category`, `currency`, and `currentPrice.value`.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\components\Searchbar.tsx</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Component:** `Searchbar`
+**Functionality:** A search bar component that takes a product URL as input, validates it against a Daraz.com domain format, and triggers a product scraping and storage process using the `scrapeAndStoreProduct` function from `@/lib/action`.
+**Key Features:**
+1. **Validation**: The component checks if the provided URL is valid by calling the `isValidDarazProductURL` function.
+2. **Submission Handling**: When the user submits the form, the `handleSubmit` function is called, which:
+	* Prevents default form submission behavior.
+	* Validates the input URL using `isValidDarazProductURL`.
+	* If invalid, displays an alert asking for a valid Daraz product URL.
+	* If valid, calls `scrapeAndStoreProduct` to scrape and store the product data.
+3. **Loading Indicator**: A loading indicator is displayed while the scraping process is in progress.
+**Props and State:**
+1. `searchPrompt`: The user-inputted search prompt (URL).
+2. `isLoading`: A state variable indicating whether the scraping process is in progress.
+This component seems to be part of a larger application, possibly using Next.js, that allows users to search for products on Daraz.com by providing a product URL as input.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\action\index.ts</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+The code is written in JavaScript and utilizes Next.js and Mongoose for server-side rendering and database interactions. It appears to be a part of an e-commerce platform that fetches and stores product data from external sources, such as Daraz (a Pakistani e-commerce website).
+**Functions**
+The code exports five functions:
+1. **`scrapeAndStoreProduct`**: Scrape a product's details from Daraz and store it in the database if it doesn't exist or update its price history if it already exists.
+2. **`getProductById`**: Retrieve a product by its ID from the database.
+3. **`getAllProducts`**: Fetch all products from the database.
+4. **`getSimilarProducts`**: Find three similar products to a given product in the database.
+5. **`addUserEmailToProduct`**: Add a user's email to a product's "users" field and send them a welcome email.
+**Database Interactions**
+The code uses Mongoose to connect to a MongoDB database, perform CRUD operations (create, read, update, delete), and use caching mechanisms (via `next/cache`) to optimize performance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\models\product.model.ts</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Mongoose Model Definition**
+The code defines a Mongoose model named `Product` using the `productSchema`.
+**Model Schema**
+The schema has 22 properties, including:
+* Identification and pricing information (e.g., `url`, `currency`, `title`)
+* Product details (e.g., `category`, `image`)
+* Pricing history (e.g., `priceHistory`)
+* User ratings and reviews (e.g., `reviewsCount`, `rateCount`, `reviewScores`)
+* Stock management (e.g., `isOutOfStock`)
+* Seller information (e.g., `sellerShopName`, `positiveSellerRating`)
+**Timestamps**
+The schema also includes timestamps (`createdAt` and `updatedAt`) by default.
+**Model Export**
+The `Product` model is exported as the default export, allowing it to be used in other parts of the application.
+Overall, this code defines a robust Mongoose model for managing product data, including pricing history, user reviews, and stock information.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\mongoose.ts</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Functionality:** Establishes a connection to a MongoDB database using Mongoose.
+**Key Features:**
+* Checks if `MONGODB_URI` environment variable is set; if not, logs an error and exits.
+* Catches any errors that occur during connection establishment.
+* If already connected, logs a message indicating the existing connection is being used instead of establishing a new one.
+* Sets up Mongoose with strict query enforcement.
+**Exported Function:** `connectToDB` - an asynchronous function that connects to the MongoDB database when called.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\nodemailer\index.ts</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+This code generates and sends email notifications using Node.js and Nodemailer. It defines notification types, generates email bodies based on these types, and sends emails to subscribers.
+**Key Components**
+1. **Notification Types**: Enumerated values (`WELCOME`, `CHANGE_OF_STOCK`, `LOWEST_PRICE`, `THRESHOLD_MET`) that determine the type of email to be sent.
+2. **`generateEmailBody` Function**: Takes a product object and notification type as input, generates an email subject and body based on the notification type, and returns them as an object.
+3. **`sendEmail` Function**: Takes an `emailContent` object (containing subject and body) and a list of email addresses (`sendTo`) as input, sends an email using Nodemailer, and logs any errors or success messages.
+**Notification Email Types**
+The code supports four types of notifications:
+1. Welcome: A welcome email with information about tracking a product.
+2. Change of Stock: An alert when a product is restocked.
+3. Lowest Price: An alert when a product reaches its lowest price ever.
+4. Threshold Met: An alert when a product's discount exceeds 40% (configurable).
+**Email Generation and Sending**
+The `generateEmailBody` function generates an email subject and body based on the notification type, using data from the provided product object. The `sendEmail` function sends an email to subscribers with the generated content.
+Overall, this code is designed to automate sending notifications about price tracking and stock changes to subscribers, using a predefined set of notification types.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\scrapper\index.ts</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Functionality:** The `scrapeDarazProduct` function scrapes product information from the Daraz e-commerce website using their proxy server.
+**Input:** A URL of a product page on Daraz.
+**Output:** An object containing product details, such as title, description, price, ratings, reviews, and more.
+**Key Features:**
+1. Authentication with Daraz's proxy server using username and password from environment variables.
+2. Parsing HTML content of the product page using Cheerio.
+3. Extracting JSON data from a script tag on the page.
+4. Converting JSON data into a structured object with various product details.
+5. Handling errors and throwing an error message if scraping fails.
+**Notes:**
+* The code uses `axios` for HTTP requests and `cheerio` for HTML parsing.
+* The function returns `undefined` if no URL is provided or if scraping fails.
+* The product details are stored in a `Product` object, which is imported from another file (`@/types/Product`).</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\lib\utils.ts</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Functionality**
+The code consists of several functions related to extracting and manipulating data from web pages. The main functionalities are:
+1. **Extracting prices**: The `extractPrice` function extracts price text from a list of elements, trims it, removes non-numeric characters, and returns the cleaned price.
+2. **Extracting currency symbols**: The `extractCurrency` function extracts the first character (assumed to be the currency symbol) from an element's text.
+3. **Extracting product descriptions**: The `extractDescription` function searches for possible elements holding a product description on a web page and returns their combined text content.
+**Additional Functions**
+The code also includes functions related to:
+1. **Price history manipulation**: The `getHighestPrice`, `getLowestPrice`, and `getAveragePrice` functions calculate the highest, lowest, and average prices from a list of price history items.
+2. **Email notification type determination**: The `getEmailNotifType` function determines the type of email notification based on the comparison between the current product's price history and the scraped product's data.
+3. **Number formatting**: The `formatNumber` function formats a number with commas as thousand separators.
+**Types**
+The code uses types imported from `"@/types"` (not shown), which likely define the structures for `Price`, `PriceHistoryItem`, and `Product` objects.
+Overall, this code seems to be designed for automating data extraction and manipulation tasks related to product prices and descriptions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\next.config.js</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Next.js Configuration**
+This code exports a Next.js configuration object (`nextConfig`) that enables:
+* Experimental server actions
+* External packages (including Mongoose) for server components
+* Image domains:
+	+ `static-01.daraz.com` and its variants
+	+ Additional image domains are commented out
+The configuration is then exported using `module.exports`.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\package-lock.json</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>This is a JSON object that represents a list of packages and their dependencies, as installed by npm (Node Package Manager). The object contains metadata about each package, including its version, resolved URL, integrity hash, and dependencies.
+The keys in the object are package names, and the corresponding values are objects with the following properties:
+* `version`: the version of the package
+* `resolved`: the resolved URL for the package
+* `integrity`: the integrity hash for the package
+* `dev`: a boolean indicating whether this is a development dependency (true) or not (false)
+* `requires`: an object with dependencies required by this package
+The packages listed in this object are likely part of a larger project, and this JSON representation is probably used to store metadata about the installed packages.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\package.json</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>**Package.json Summary**
+This is a `package.json` file, which is the primary configuration file for Node.js projects.
+**Project Information**
+* Project name: darazscan
+* Version: 0.1.0
+* Private flag set to true (indicates this is likely a local development project)
+**Scripts**
+The project has four scripts defined:
+* `dev`: Runs the Next.js dev server
+* `build`: Builds the Next.js application for production
+* `start`: Starts the Next.js server in production mode
+* `lint`: Runs code linting using Next.js's built-in linter
+**Dependencies**
+The project relies on several dependencies, including:
+* Front-end libraries: React, React DOM, React Responsive Carousel, Headless UI React
+* Server-side modules: Mongoose (for MongoDB interactions), Axios (for HTTP requests), Nodemailer (for email sending)
+* Utilities: Supports-Color for color management
+**Dev Dependencies**
+The project has several development dependencies:
+* TypeScript and related type definitions
+* Autoprefixer and PostCSS for CSS preprocessing
+* Tailwind CSS for styling
+Overall, this project appears to be a Next.js application with a focus on server-side rendering, using MongoDB and email sending features. The code is written in TypeScript, and the project uses various front-end libraries and utilities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\postcss.config.js</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>This code exports an object that configures plugins for a CSS or JavaScript project. Specifically, it enables:
+1. Tailwind CSS
+2. Autoprefixer
+Both plugins are likely used to enhance and standardize CSS output in the project. No further details about the project's specifics or functionality are provided by this snippet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\tailwind.config.ts</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>This code is a Tailwind CSS configuration file. Here's a summary of its contents:
+**Content**: The content specifies which files in the project to scan for utility classes. It includes pages, components, and app files with JavaScript, TypeScript, JSX, TSX, and MDX extensions.
+**Theme**: The theme defines custom colors, shadows, max-widths, font families, and border radii. Specifically:
+* Custom color palette with primary, secondary, gray, white, black, and neutral-black shades.
+* A custom box shadow style called "xs".
+* A custom max-width style called "10xl" set to 1440px.
+* Two custom font family styles: Inter and Space Grotesk.
+* A custom border radius style called "10" set to 10px.
+**Plugins**: There are no plugins enabled in this configuration file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\tsconfig.json</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>**Configuration File Summary**
+This is a configuration file for a JavaScript compiler, specifically targeting ES5. The main settings are:
+* **Target**: ES5
+* **Module system**: ESNext with ES6+ module resolution
+* **Compiler plugins**: Using the "next" plugin
+* **Paths**: Mapping the `@` alias to the current directory (`.`)
+The file also specifies which files to include or exclude from compilation:
+* **Include**: Typescript (.ts, .tsx), Next.js environment configuration (next-env.d.ts), and types in the `.next/types` directory.
+* **Exclude**: The `node_modules` directory.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\types\index.ts</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Data Models**
+The code defines several data models using TypeScript types, including:
+* `PriceHistoryItem`: an object with a single property `price` of type `Price`.
+* `User`: an object with a single property `email` of type string.
+* `Product`: an object with numerous properties, including:
+	+ Details about the product (id, url, currency, image, title, etc.)
+	+ Pricing information (current price, original price, lowest/highest/average prices)
+	+ Review and rating data
+	+ Seller information
+* `NotificationType`: a union type with four possible values ("WELCOME", "CHANGE_OF_STOCK", "LOWEST_PRICE", "THRESHOLD_MET").
+* `EmailContent` and `EmailProductInfo`: objects used to represent email content, each with two properties (subject and body).
+* `Price`: an object with two properties (`text` and `value`) representing a price value.
+**Notable Features**
+The code uses TypeScript types to define strict data structures for various models. It also includes type annotations for several fields, indicating that they are optional or have specific data types (e.g., string, number).</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper\vercel.json</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>This code defines a single cron job configuration. Here's a summary:
+**Key Information:**
+* The cron job is located at the path `/api/cron`.
+* It is scheduled to run every day at 1:30 PM (13:30 hours) minute 30.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore:Updated global variables and caching in Flask API endpoints for project badge, image, languages, and name
</commit_message>
<xml_diff>
--- a/output/Daraz_Scraper_api_reference_data.xlsx
+++ b/output/Daraz_Scraper_api_reference_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1080,6 +1080,707 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\.env.local.copy</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>It appears you haven't provided any code yet. Please paste the code you'd like me to summarize, and I'll be happy to assist!</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\.gitignore</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>This code is a `.gitignore` file, which specifies files and directories to be ignored by Git. In other words, it tells Git not to track or include these specific files in its repository.
+The file lists various categories of files to ignore:
+1. **Dependencies**: `node_modules`, `.pnp`, and `.pnp.js` files.
+2. **Testing**: `/coverage` directory.
+3. **Next.js**: `.next/` directory and `/out/` directory.
+4. **Production**: `/build` directory.
+5. **Miscellaneous**:
+	* Apple-specific file `D.S_Store`
+	* SSL certificates in PEM format
+6. **Debugging**:
+	* Various log files generated by npm and yarn package managers (`npm-debug.log`, etc.)
+7. **Local environment variables**: `.env*.local` files.
+8. **Vercel**: `.vercel` directory ( likely for Vercel's serverless platform).
+9. **TypeScript**: `*.tsbuildinfo` file (likely a build artifact) and `next-env.d.ts` file.
+By ignoring these files, Git won't include them in the repository, which helps keep the repository size smaller and more manageable.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\README.md</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Here's a summary of the code:
+**Project Overview**
+DarazScrapper is a Next.js application that scrapes product details from Daraz, tracks price changes, and notifies users when specific conditions are met. It uses MongoDB for data storage and Bright Data for efficient scraping.
+**Key Features**
+1. **Price Tracking**: Records highest and lowest prices for products over time.
+2. **Notification System**: Sends alerts when price drops below a set threshold.
+3. **Web Scraping**: Extracts product details like name, price, and rating.
+4. **Cron Jobs**: Schedules scraping tasks to run periodically.
+**Technologies Used**
+1. Next.js
+2. MongoDB
+3. Bright Data
+4. Node.js
+5. Tailwind CSS
+**Installation and Usage**
+1. Clone the repository and install dependencies.
+2. Set up environment variables for MongoDB, Bright Data, and email services.
+3. Start the development server.
+4. Add product URLs to scrape and track price changes.
+**Contribution and License**
+Contributions are welcome! The project is licensed under the MIT License.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\app\api\cron\route.ts</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+The code exports an API endpoint that runs a cron job to scrape product data from Daraz, update the database, and send email notifications accordingly.
+**Main Functionality**
+1. Connects to the database using `connectToDB`.
+2. Retrieves all products from the database.
+3. Scrape latest product details for each product using `scrapeDarazProduct` and updates the database with the new information.
+4. For each product, determines the email notification type using `getEmailNotifType` and sends an email to users who have subscribed to that product's notifications using `sendEmail`.
+5. Returns a JSON response with a success message and the updated products.
+**Additional Features**
+* The API endpoint is configured as dynamic with revalidation set to 0.
+* The function has a maximum duration of 5 minutes (300 seconds).
+* The code uses a `Promise.all` to update multiple products in parallel, improving performance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\app\globals.css</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>**Summary of Code**
+The provided code is a Tailwind CSS configuration file that defines various utility classes for styling HTML elements. It includes:
+1. **Global styles**: A reset of global styles, setting `margin`, `padding`, and `box-sizing` to their default values.
+2. **Font family**: Setting the font family to "Inter" using the `@layer base` directive.
+**Utility Classes**
+The code defines several utility classes for styling various HTML elements:
+1. **Button**: `.btn` class with styles for a button, including background color, hover effect, and text styles.
+2. **Headline**: `.head-text` class with styles for a large headline, including font size, leading, tracking, and text color.
+3. **Section Text**: `.section-text` class with styles for a section text element, including font size and style.
+4. **Small Text**: `.small-text` class with styles for small text elements, including font size and style.
+**Component-Specific Styles**
+The code also defines several component-specific utility classes:
+1. **Hero Carousel**: `.hero-carousel` class with styles for a hero carousel element.
+2. **Carousel**: `.carousel` class with styles for a carousel element.
+3. **Product Details Page**: Various classes for styling product details page elements, including `.product-container`, `.product-image`, and `.product-info`.
+4. **Modal**: Classes for styling a modal dialog, including `.dialog-container` and `.dialog-content`.
+5. **Navbar**: Class for styling a navbar, including `.nav`.
+6. **Price Info**: Class for styling price info elements.
+7. **Product Card**: Classes for styling product card elements.
+8. **Searchbar Input**: Classes for styling searchbar input elements.
+Overall, this code provides a set of reusable utility classes and component-specific styles to simplify the process of styling HTML elements using Tailwind CSS.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\app\layout.tsx</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Next.js Page Layout**
+This code defines a basic layout for a Next.js page. It imports two Google fonts, `Inter` and `Space_Grotesk`, and sets them up for use in the application.
+The code then exports metadata for the page, including a title and description.
+Finally, it defines a `RootLayout` component that wraps around the page's content (`children`). This layout includes:
+* An `&lt;html&gt;` element with a `lang` attribute set to "en"
+* A `&lt;body&gt;` element with a class name set to the `Inter` font's CSS class
+* A `&lt;main&gt;` element with a maximum width of 10xl and centered horizontally
+* A `Navbar` component (imported from another file) rendered inside the `&lt;main&gt;` element
+Overall, this code sets up a basic template for a Next.js page that uses two fonts and includes a navbar at the top.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\app\page.tsx</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+This is a React component named `Home` that renders the homepage content. It uses several components from other files, including `HeroCarousel`, `ProductCard`, and `Searchbar`.
+**Features**
+1. **Hero Section**: A section at the top with a call-to-action (CTA) text, an icon, and a hero carousel.
+2. **Trending Products**: A section displaying trending products fetched from the server using the `getAllProducts` function.
+3. **Product Cards**: Each product is displayed as a card with details fetched from the server.
+**Imported Components**
+* `HeroCarousel`
+* `ProductCard`
+* `Searchbar`
+* `Image`
+**Server-Side Functionality**
+The component uses an async function `getAllProducts` to fetch all products from the server and store them in the `allProducts` variable. The fetched data is then used to render the product cards.
+Overall, this code snippet appears to be part of a larger e-commerce platform, showcasing trending products with a hero carousel and search functionality.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\app\products\[id]\page.tsx</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+The code defines a React component named `ProductDetails` that displays detailed information about a specific product. The product's ID is passed as a parameter to the component.
+**Components Used**
+The component uses several other components, including:
+* `PriceInfoCard`: a reusable card component for displaying price-related information
+* `ProductCard`: a reusable card component for displaying individual products
+* `Modal`: a modal window component that can be used to display additional information
+**Functionality**
+The component performs the following functions:
+1. Retrieves product data from an API using the `getProductById` function.
+2. If the product is not found, redirects to the root URL (`"/"`).
+3. Retrieves similar products from the API using the `getSimilarProducts` function.
+4. Displays the product's image, title, category, and other information in a card layout.
+5. Displays the product's current price, average price, highest price, lowest price, and discount rate.
+6. Displays a button to buy now or visit the shop.
+7. If similar products are available, displays them in a grid layout.
+**Features**
+The component also includes several features, such as:
+* A modal window that can be opened by clicking on a button
+* Social proof indicators (e.g., heart icon for rating)
+* Seller information and shop link
+* Buy now and visit shop buttons
+Overall, the `ProductDetails` component is designed to display detailed information about a specific product, along with relevant additional features.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\HeroCarousel.tsx</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>**Code Summary**
+This code snippet is a React component that renders a carousel of hero images on a website. Here's a breakdown:
+* **Imports**: The code imports necessary libraries, including `React`, `react-responsive-carousel` for the carousel functionality, and `next/image` for image handling.
+* **Hero Images Array**: An array of objects (`heroImages`) is defined to store image metadata (URLs, alt text).
+* **HeroCarousel Component**: A React functional component (`HeroCarousel`) is created that returns a JSX element containing:
+	+ An absolute positioned arrow icon at the bottom left corner.
+	+ A carousel container that loops through the `heroImages` array and renders each image as an `Image` component from `next/image`.
+* **Carousel Configuration**: The carousel settings are defined, including:
+	+ Disabling thumbs and arrows for a clean design.
+	+ Auto-playing and infinite looping with a 2-second interval.
+	+ Hiding status information.
+This code is designed to display a slideshow of product hero images on a website.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\Modal.tsx</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Here's a summary of the code:
+**Modal Component**
+The code defines a React component called `Modal` that displays a modal dialog with a form to collect an email address from users. The component is designed to be used in a Next.js application.
+**Functionality**
+When clicked, the "Track" button opens the modal dialog, which contains:
+1. A logo and a close button
+2. A header text and a paragraph of text explaining the purpose of the modal
+3. A form with an input field for entering an email address and a submit button
+When the submit button is clicked, the `handleSubmit` function is called, which:
+1. Prevents the default form submission behavior
+2. Sets a loading state to true
+3. Calls the `addUserEmailToProduct` API function to add the entered email address to a product (identified by the `productId` prop)
+4. Resets the loading state and clears the input field
+**Props**
+The component expects a single prop, `productId`, which is used to identify the product being tracked.
+**State Management**
+The component uses React's built-in `useState` hook to manage three pieces of state:
+1. `isOpen`: A boolean indicating whether the modal is open
+2. `isSubmitting`: A boolean indicating whether the form submission is in progress
+3. `email`: The value entered into the input field
+**Transitions**
+The code uses Headless UI's `Transition` component to smoothly animate the opening and closing of the modal dialog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\Navbar.tsx</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Code Summary**
+The provided code defines a reusable React component called `Navbar`. The component renders a navigation bar with a logo, links, and icons.
+**Key Features**
+* The component uses Next.js's built-in `Link` component to create a link back to the homepage.
+* It includes an array of icon objects (`navIcons`) that are mapped over to render individual icons.
+* Each icon is rendered as an `Image` component from Next.js, with a specified source URL and alt text.
+* The navbar has a fixed width and contains a logo, a link to the homepage, and a list of navigation icons.
+**Export**
+The `Navbar` component is exported as the default export of the file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\PriceInfoCard.tsx</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Component:** `PriceInfoCard`
+**Purpose:** Displays a card with title, icon, and value information.
+**Props:**
+* `title`: string (card title)
+* `iconSrc`: string (URL of icon to display)
+* `value`: string (displayed value)
+**Structure:**
+* A `&lt;div&gt;` container with class `price-info_card`
+* A paragraph displaying the `title` text
+* An image element displaying the `iconSrc` icon
+* A paragraph displaying the `value` text in a larger font size and color</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\ProductCard.tsx</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>**Code Summary**
+The provided code defines a reusable React component called `ProductCard`. This component displays information about a single product, including:
+1. **Image**: A product image fetched from the `product.image` prop.
+2. **Title**: The product title displayed in an `&lt;h3&gt;` tag.
+3. **Categories**: The first two categories assigned to the product (comma-separated).
+4. **Price**: The current price of the product, formatted with currency symbol and value.
+The component uses Next.js's built-in `Link` component to create a link to the product details page based on the `product._id`. It also utilizes the `Image` component from `next/image` for image rendering.
+**Props**
+The component expects a single prop: `product`, which is an object of type `Product` (imported from `/@/types`). This prop contains all the necessary information about the product to be displayed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\components\Searchbar.tsx</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Component:** `Searchbar`
+**Purpose:** To allow users to enter a Daraz product URL, validate it, and then scrape and store the product information using the `scrapeAndStoreProduct` function. The user is redirected to a new page with the product ID.
+**Key Features:**
+1. Validation of input URL using the `isValidDarazProductURL` function.
+2. Form submission handling via the `handleSubmit` function, which calls `scrapeAndStoreProduct` and redirects the user to a new page with the product ID.
+3. Display of loading indicator while scraping and storing product information.
+4. Error handling for invalid input URLs.
+**State Management:**
+* `searchPrompt`: stores the user's input URL.
+* `isLoading`: indicates whether the form is being submitted or not.
+* `router` from `next/navigation`: used to redirect the user to a new page with the product ID.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\action\index.ts</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Functionality**
+The code provides a set of functions for interacting with a MongoDB database to manage products and users.
+**Functions**
+1. **`scrapeAndStoreProduct`**: Scrapes product information from Daraz, stores it in the database, and updates price history if the product already exists.
+2. **`getProductById`**: Retrieves a product by its ID.
+3. **`getAllProducts`**: Returns all products in the database.
+4. **`getSimilarProducts`**: Finds similar products (up to 3) based on the current product's ID.
+5. **`addUserEmailToProduct`**: Adds a user email to a product, generates an email content, and sends it to the user if they don't already exist.
+**Assumptions**
+* The code assumes the presence of a MongoDB database connection (established via `connectToDB`) and Next.js caching (via `revalidatePath`).
+* It also relies on external functions (`getAveragePrice`, `getHighestPrice`, `getLowestPrice`, `scrapeDarazProduct`, `generateEmailBody`, `sendEmail`) which are not provided in the code snippet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\models\product.model.ts</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Overview**
+This code defines a Mongoose schema for a MongoDB database, specifically designed to store product information. The schema is then used to create a model called `Product`.
+**Fields**
+The schema includes the following fields:
+* General product details:
+	+ URL
+	+ Currency
+	+ Image
+	+ Title
+	+ Category (an array of strings)
+* Pricing and sales data:
+	+ Current price with text and value
+	+ Original price with text and value
+	+ Price history (array of objects with date and price)
+	+ Discount rate
+* Reviews and ratings:
+	+ Reviews count
+	+ Rate count
+	+ Review scores (array of numbers)
+* Inventory management:
+	+ Product quantity value
+	+ Is out of stock (boolean, defaulting to false)
+* Seller information:
+	+ Product brand
+	+ Shop name
+	+ Shop URL
+	+ Positive seller rating
+* User data:
+	+ Users (array of objects with email)
+* Calculated prices:
+	+ Lowest price with text and value
+	+ Highest price with text and value
+	+ Average price with text and value
+**Model Creation**
+The schema is then used to create a Mongoose model called `Product`, which can be used to interact with the MongoDB database.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\mongoose.ts</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>**Database Connection Module**
+This module connects to a MongoDB database using the Mongoose library. Here's a summary of its functionality:
+* It checks if an environment variable `MONGODB_URI` is defined, and exits with an error message if it's not.
+* If a connection already exists (`isConnected` flag), it logs a message indicating that an existing connection will be used instead of establishing a new one.
+* Otherwise, it attempts to connect to the MongoDB database using the provided URI. If successful, it sets `isConnected` to `true` and logs a success message.
+* If the connection attempt fails, it catches the error and logs it for debugging purposes.
+**Exported Function:**
+The module exports a single function `connectToDB`, which is an asynchronous function that establishes a connection to the MongoDB database.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\nodemailer\index.ts</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Purpose:** This Node.js script sends automated emails to users based on product tracking notifications.
+**Key Features:**
+1. **Notification Types:** The script supports four notification types:
+	* `WELCOME`: Welcomes the user to the service.
+	* `CHANGE_OF_STOCK`: Notifies when a tracked product is restocked.
+	* `LOWEST_PRICE`: Alerts the user when a tracked product reaches its lowest price.
+	* `THRESHOLD_MET`: Notifies when a tracked product meets a specified discount threshold (40% in this case).
+2. **Email Generation:** The script uses templates to generate email bodies based on the notification type and product information.
+3. **Email Sending:** The script uses Nodemailer to send emails to users via a Hotmail service.
+**Key Functions:**
+1. `generateEmailBody`: Generates an email body based on the notification type, product info, and other parameters.
+2. `sendEmail`: Sends an email to one or more recipients using the generated email body and other configuration settings.
+Overall, this script provides a basic implementation of automated email sending for product tracking notifications.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\scrapper\index.ts</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>**Scraping Function Summary**
+The `scrapeDarazProduct` function is an asynchronous function that extracts product information from the Daraz website. It takes a URL as input and returns a `Product` object or `undefined`.
+Here's what it does:
+1. **Authentication**: The function uses environment variables to authenticate with the Bright Data proxy service.
+2. **Request**: It sends a GET request to the provided URL using Axios, passing authentication details.
+3. **Cheerio Parsing**: The response data is parsed using Cheerio to extract JavaScript code.
+4. **JSON Extraction**: A regular expression is used to find a specific script content, which is then JSON-parsed to extract product information.
+5. **Product Data Extraction**: Various fields are extracted from the JSON object, including:
+	* Seller details
+	* Product rating and review count
+	* Product brand, title, description, categories, image, and URL
+	* Price history and discount rate
+	* Reviews scores and counts
+6. **Return**: The function returns a `Product` object containing the extracted data.
+**Error Handling**
+The function catches any errors that occur during execution and throws a new error with a descriptive message.
+Note: This summary is based on the provided code snippet, but it's essential to review the full code for completeness and accuracy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\lib\utils.ts</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Functions**
+1. `extractPrice`: Extracts and returns the price from a list of possible elements. It iterates over each element, extracts the text, trims it, and removes non-numeric characters to get the clean price. If no valid price is found, an empty string is returned.
+2. `extractCurrency`: Extracts and returns the currency symbol from an element by taking the first character of its trimmed text.
+3. `extractDescription`: Extracts and returns the description from two possible elements (`.a-unordered-list .a-list-item` and `.a-expander-content p`). If no matching elements are found, an empty string is returned.
+4. `getHighestPrice`, `getLowestPrice`, and `getAveragePrice`: These functions calculate and return the highest, lowest, or average price from a list of price history items.
+5. `getEmailNotifType`: Returns the notification type based on the comparison between scraped product and current product prices, stock status, and discount rate.
+**Utilities**
+1. `Notification` object: Defines constants for different types of notifications (WELCOME, CHANGE_OF_STOCK, LOWEST_PRICE, THRESHOLD_MET).
+2. `THRESHOLD_PERCENTAGE`: A constant representing the threshold percentage (40) used to determine if a product's discount rate meets the notification condition.
+3. `formatNumber`: A function that formats a number as a string with a locale-independent format.
+**Purpose**
+The code appears to be part of a web scraping or data extraction project, where prices and other product information are being extracted from various elements on a website (e.g., Daraz). The functions provided help process this data and calculate relevant statistics, such as highest/lowest prices, average price, and notification types.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\next.config.js</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Next.js Configuration**
+This code exports a Next.js configuration object (`nextConfig`) that enables experimental features and specifies image domains.
+* Enables experimental server actions and allows external packages from `mongoose`.
+* Specifies allowed image domains:
+	+ `static-01.daraz.com` (and its subdomain)
+	+ `static-01.daraz.com.np` and `np-live-21.slatic.net`
+The code exports this configuration as a module, making it available to Next.js.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\package-lock.json</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>This is a JSON object that appears to be the output of `npm ls` command, which lists all the dependencies of a project.
+Here are some key points from this output:
+* The project has 22 dependencies.
+* Some notable dependencies include:
+	+ Express.js (version 4.17.1)
+	+ Webpack (version 5.38.0)
+	+ Browserslist (version 4.26.2)
+	+ Whatwg-url (version 11.0.0)
+	+ Watchpack (version 2.4.0)
+* The project also has some dev dependencies, including:
+	+ ESLint (version 8.3.0)
+	+ Babel-core (version 7.0.0-beta.55)
+	+ Webpack-cli (version 3.3.10)
+This output can be useful for identifying and managing the dependencies of a project, such as updating versions or removing unused packages.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\package.json</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Package File**
+This is a `package.json` file, which defines metadata and dependencies for a JavaScript project.
+**Project Information**
+* Project name: darazscan
+* Version: 0.1.0
+* Private package (not intended to be published): true
+**Scripts**
+The project has four scripts defined:
+* dev: runs the development server with `next dev`
+* build: builds the application with `next build`
+* start: starts the production server with `next start`
+* lint: runs code linters with `next lint`
+**Dependencies**
+The project depends on several packages, including:
+* Front-end libraries (React, Next.js)
+* Back-end dependencies (Mongoose, Nodemailer)
+* Utilities and plugins (Axios, Cheerio)
+**Development Dependencies**
+The project has additional dependencies for development purposes, including:
+* TypeScript and its type definitions
+* Autoprefixer and PostCSS for CSS processing
+* Tailwind CSS for styling</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\postcss.config.js</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>This code exports a configuration module for a JavaScript project, specifically setting up two CSS preprocessors:
+* `tailwindcss`: enables Tailwind CSS styling
+* `autoprefixer`: adds vendor prefixes to CSS rules for cross-browser compatibility
+In summary, this code sets up the necessary configurations for using Tailwind CSS and Autoprefixer in a project.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\tailwind.config.ts</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+This is a Tailwind CSS configuration file. It defines the following settings:
+* **Content**: Specifies the files and directories that will be scanned for utility classes to generate styles.
+* **Theme**:
+	+ Extends the default theme with custom color palette (primary, secondary, grays, whites, blacks).
+	+ Defines box shadow effects.
+	+ Sets maximum widths for containers.
+	+ Specifies font families.
+	+ Customizes border radius values.
+* **Plugins**: Currently empty.
+Overall, this configuration file sets up a customized Tailwind CSS theme with specific colors, styles, and layout settings.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\tsconfig.json</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Here is a summary of the provided code:
+**Webpack Configuration**
+This configuration file defines settings for a Webpack build process. The main features include:
+* **ES5 target**: Compile JavaScript to ES5 syntax.
+* **Strict mode**: Enable strict type checking and other safety features.
+* **JSX preservation**: Preserve JSX syntax in compiled output.
+* **Module resolution**: Use the "bundler" strategy to resolve module imports.
+* **Incremental builds**: Allow incremental rebuilds for faster development.
+**File inclusion/exclusion**
+The configuration specifies which files to include or exclude from the build process:
+* Include: `next-env.d.ts`, all `.ts` and `.tsx` files, and TypeScript definitions in the `.next/types` directory.
+* Exclude: The entire `node_modules` directory.
+**Plugin usage**
+A single plugin is enabled: "next", which likely provides features specific to Next.js projects.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\types\index.ts</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Here is a summary of the code:
+**Data Types**
+The code defines several data types to represent various pieces of information in an e-commerce application.
+* **PriceHistoryItem**: An object containing a single price field.
+* **User**: An object with a single email field.
+* **Product**: A complex object representing a product, including fields for:
+	+ Basic product info (ID, URL, currency, image, title, category)
+	+ Prices and discounts (current and original prices, discount rate)
+	+ Product details (description, reviews count, rating, scores)
+	+ Seller information (brand, shop name, URL, rating)
+	+ Historical price data (price history array or empty array)
+* **NotificationType**: An enum with four possible values representing different types of notifications.
+* **EmailContent**: An object containing a subject and body for an email.
+* **EmailProductInfo**: An object with title and URL fields to display product information in an email.
+* **Price**: A simple object with text and value fields to represent a price.
+**Notes**
+The code uses TypeScript syntax and appears to be designed for use in a Node.js or MongoDB environment. The `default` field in the `Product` type is likely a placeholder and should be removed or replaced with actual data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Github_repos\Daraz_Scraper.git\vercel.json</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>This JSON code defines a single cron job schedule. Here's a breakdown:
+* The top-level object contains an array of crons, with only one cron job defined.
+* The cron job has two properties:
+	+ `path`: specifies the API endpoint for this cron job, which is `/api/cron`.
+	+ `schedule`: defines the timing of the cron job using the standard cron format (minute, hour, day of month, month, day of week). In this case, it runs every day at 13:30 (1:30 PM) UTC time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>